<commit_message>
changes to get luis's photo to rotate
</commit_message>
<xml_diff>
--- a/public/img/ads.img/ExcelDatabase.xlsx
+++ b/public/img/ads.img/ExcelDatabase.xlsx
@@ -86,9 +86,6 @@
     <t>5.jpeg</t>
   </si>
   <si>
-    <t>awesome</t>
-  </si>
-  <si>
     <t>not so awesome</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Babylon dictionary</t>
+  </si>
+  <si>
+    <t>awesomeness</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,16 +539,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -588,10 +588,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>1</v>

</xml_diff>